<commit_message>
chore: update internal Excel template for improved data handling
</commit_message>
<xml_diff>
--- a/public/plantillas/int_excel_template.xlsx
+++ b/public/plantillas/int_excel_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\BOLT MAT89\DOC - HTML - PDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\mat89\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CFCBD2-BE72-446E-B9E7-FD16C698FA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DA1613-A037-4007-B4F2-E742ED483C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A836C92A-72EE-4D4A-871D-9A1A52BD3A60}"/>
   </bookViews>
@@ -165,10 +165,10 @@
     <t>{nenv}</t>
   </si>
   <si>
-    <t>{almacen}</t>
-  </si>
-  <si>
     <t>{fecha_envio}+15</t>
+  </si>
+  <si>
+    <t>{alm_envia}</t>
   </si>
 </sst>
 </file>
@@ -991,7 +991,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,13 +1126,13 @@
         <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>25</v>
@@ -1159,13 +1159,13 @@
         <v>40</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="4"/>

</xml_diff>

<commit_message>
chore: update internal Excel template for improved functionality
</commit_message>
<xml_diff>
--- a/public/plantillas/int_excel_template.xlsx
+++ b/public/plantillas/int_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\mat89\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFFF5DA-83EB-488C-9193-B481F28057BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2101AC8-BCFD-4277-9AE0-D6F36318AFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A836C92A-72EE-4D4A-871D-9A1A52BD3A60}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>POS</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>{alm_envia}</t>
+  </si>
+  <si>
+    <t>{fecha_necesidad}</t>
   </si>
 </sst>
 </file>
@@ -341,17 +344,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -988,7 +987,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,105 +1008,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="10"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="11" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="J2" s="28" t="s">
+      <c r="G2" s="11"/>
+      <c r="J2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="F3" s="13"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="9.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1128,19 +1127,19 @@
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>36</v>
+      <c r="H7" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="21"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1161,17 +1160,17 @@
       <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>36</v>
+      <c r="H8" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="21"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>3</v>
       </c>
       <c r="B9" s="1"/>
@@ -1180,301 +1179,301 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="21"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="20"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>4</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="21"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="20"/>
     </row>
     <row r="11" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>5</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="21"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="20"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>6</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="21"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>7</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="21"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>8</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="21"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="20"/>
     </row>
     <row r="15" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20">
+      <c r="A15" s="19">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="21"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20">
+      <c r="A16" s="19">
         <v>10</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="21"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>11</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="21"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>12</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="21"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>13</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="21"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
+      <c r="A20" s="19">
         <v>14</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="21"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="20"/>
     </row>
     <row r="21" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20">
+      <c r="A21" s="19">
         <v>15</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="21"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
+      <c r="A22" s="19">
         <v>16</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="21"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
+      <c r="A23" s="19">
         <v>17</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="21"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+      <c r="A24" s="19">
         <v>18</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="21"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
+      <c r="A25" s="19">
         <v>19</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="21"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="26" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
+      <c r="A26" s="19">
         <v>20</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="21"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="20"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
quitado merge en plantilla excel
</commit_message>
<xml_diff>
--- a/public/plantillas/int_excel_template.xlsx
+++ b/public/plantillas/int_excel_template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\mat89\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9B571-F82F-44B0-9845-0A8FB0F43834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB023C1-C0AA-4A4E-A26E-0EB4D1DF8209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A836C92A-72EE-4D4A-871D-9A1A52BD3A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -233,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -284,32 +284,6 @@
         <color rgb="FF800080"/>
       </left>
       <right/>
-      <top style="thick">
-        <color rgb="FF800080"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF800080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF800080"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF800080"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF800080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF800080"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -329,12 +303,19 @@
       <left style="thick">
         <color rgb="FF800080"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF800080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thick">
         <color rgb="FF800080"/>
       </right>
-      <top style="thin">
-        <color rgb="FF800080"/>
-      </top>
+      <top/>
       <bottom style="thick">
         <color rgb="FF800080"/>
       </bottom>
@@ -344,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -370,7 +351,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -381,11 +362,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -419,15 +397,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -987,7 +963,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,18 +985,18 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
@@ -1028,30 +1004,30 @@
         <v>36</v>
       </c>
       <c r="G2" s="11"/>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1059,54 +1035,54 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="9.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="E5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1127,7 +1103,7 @@
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1136,10 +1112,10 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="20"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <v>2</v>
       </c>
       <c r="B8" s="1"/>
@@ -1148,15 +1124,15 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="18"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="20"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>3</v>
       </c>
       <c r="B9" s="1"/>
@@ -1170,10 +1146,10 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="20"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>4</v>
       </c>
       <c r="B10" s="4"/>
@@ -1187,10 +1163,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="20"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>5</v>
       </c>
       <c r="B11" s="4"/>
@@ -1204,10 +1180,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="20"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>6</v>
       </c>
       <c r="B12" s="4"/>
@@ -1221,10 +1197,10 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="20"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>7</v>
       </c>
       <c r="B13" s="4"/>
@@ -1238,10 +1214,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="20"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="A14" s="18">
         <v>8</v>
       </c>
       <c r="B14" s="4"/>
@@ -1255,10 +1231,10 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="20"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>9</v>
       </c>
       <c r="B15" s="4"/>
@@ -1272,10 +1248,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="20"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>10</v>
       </c>
       <c r="B16" s="4"/>
@@ -1289,10 +1265,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
@@ -1306,10 +1282,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="20"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>12</v>
       </c>
       <c r="B18" s="4"/>
@@ -1323,10 +1299,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="19"/>
     </row>
     <row r="19" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
@@ -1340,10 +1316,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="20"/>
+      <c r="M19" s="19"/>
     </row>
     <row r="20" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>14</v>
       </c>
       <c r="B20" s="4"/>
@@ -1357,10 +1333,10 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <v>15</v>
       </c>
       <c r="B21" s="4"/>
@@ -1374,10 +1350,10 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="20"/>
+      <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
+      <c r="A22" s="18">
         <v>16</v>
       </c>
       <c r="B22" s="4"/>
@@ -1391,10 +1367,10 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="20"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="A23" s="18">
         <v>17</v>
       </c>
       <c r="B23" s="4"/>
@@ -1408,10 +1384,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="20"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="A24" s="18">
         <v>18</v>
       </c>
       <c r="B24" s="4"/>
@@ -1425,10 +1401,10 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="20"/>
+      <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19">
+      <c r="A25" s="18">
         <v>19</v>
       </c>
       <c r="B25" s="4"/>
@@ -1442,10 +1418,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="20"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19">
+      <c r="A26" s="18">
         <v>20</v>
       </c>
       <c r="B26" s="4"/>
@@ -1459,17 +1435,17 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="20"/>
+      <c r="M26" s="19"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <mergeCells count="3">
     <mergeCell ref="B1:D3"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation showErrorMessage="1" error="Elige un Taller destino de la lista" sqref="C4:D4" xr:uid="{5806ACDB-7034-4B0E-AA6D-B6864DEB3E7B}"/>
+    <dataValidation showErrorMessage="1" error="Elige un Taller destino de la lista" sqref="D4" xr:uid="{5806ACDB-7034-4B0E-AA6D-B6864DEB3E7B}"/>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
ultimos retoques plantilla excel
</commit_message>
<xml_diff>
--- a/public/plantillas/int_excel_template.xlsx
+++ b/public/plantillas/int_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\mat89\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB023C1-C0AA-4A4E-A26E-0EB4D1DF8209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E131DB8-3910-4539-A20F-57E8EE1390AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A836C92A-72EE-4D4A-871D-9A1A52BD3A60}"/>
   </bookViews>
@@ -233,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -251,10 +251,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF800080"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -263,25 +278,18 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color rgb="FF800080"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF800080"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF800080"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -290,34 +298,54 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color rgb="FF800080"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color rgb="FF800080"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF800080"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color rgb="FF800080"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color rgb="FF800080"/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thick">
-        <color rgb="FF800080"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -325,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -347,64 +375,81 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,7 +1008,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,105 +1029,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="J2" s="24" t="s">
+      <c r="G2" s="15"/>
+      <c r="J2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
       <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="26"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="9.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="12"/>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+      <c r="B5" s="16"/>
+      <c r="C5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="10">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1103,7 +1148,7 @@
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="9" t="s">
         <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1112,10 +1157,10 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="19"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="10">
         <v>2</v>
       </c>
       <c r="B8" s="1"/>
@@ -1124,15 +1169,15 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="19"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="10">
         <v>3</v>
       </c>
       <c r="B9" s="1"/>
@@ -1146,10 +1191,10 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="19"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
+      <c r="A10" s="10">
         <v>4</v>
       </c>
       <c r="B10" s="4"/>
@@ -1163,10 +1208,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="19"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
       <c r="B11" s="4"/>
@@ -1180,10 +1225,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="19"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+      <c r="A12" s="10">
         <v>6</v>
       </c>
       <c r="B12" s="4"/>
@@ -1197,10 +1242,10 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="19"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
+      <c r="A13" s="10">
         <v>7</v>
       </c>
       <c r="B13" s="4"/>
@@ -1214,10 +1259,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="19"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
+      <c r="A14" s="10">
         <v>8</v>
       </c>
       <c r="B14" s="4"/>
@@ -1231,10 +1276,10 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="19"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
+      <c r="A15" s="10">
         <v>9</v>
       </c>
       <c r="B15" s="4"/>
@@ -1248,10 +1293,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="19"/>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
+      <c r="A16" s="10">
         <v>10</v>
       </c>
       <c r="B16" s="4"/>
@@ -1265,10 +1310,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="19"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="A17" s="10">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
@@ -1282,10 +1327,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="19"/>
+      <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
+      <c r="A18" s="10">
         <v>12</v>
       </c>
       <c r="B18" s="4"/>
@@ -1299,10 +1344,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="19"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
+      <c r="A19" s="10">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
@@ -1316,10 +1361,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="19"/>
+      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
+      <c r="A20" s="10">
         <v>14</v>
       </c>
       <c r="B20" s="4"/>
@@ -1333,10 +1378,10 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="19"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
+      <c r="A21" s="10">
         <v>15</v>
       </c>
       <c r="B21" s="4"/>
@@ -1350,10 +1395,10 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="19"/>
+      <c r="M21" s="11"/>
     </row>
     <row r="22" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
+      <c r="A22" s="10">
         <v>16</v>
       </c>
       <c r="B22" s="4"/>
@@ -1367,10 +1412,10 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="19"/>
+      <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
+      <c r="A23" s="10">
         <v>17</v>
       </c>
       <c r="B23" s="4"/>
@@ -1384,10 +1429,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="19"/>
+      <c r="M23" s="11"/>
     </row>
     <row r="24" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18">
+      <c r="A24" s="10">
         <v>18</v>
       </c>
       <c r="B24" s="4"/>
@@ -1401,10 +1446,10 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="19"/>
+      <c r="M24" s="11"/>
     </row>
     <row r="25" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
+      <c r="A25" s="10">
         <v>19</v>
       </c>
       <c r="B25" s="4"/>
@@ -1418,10 +1463,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="19"/>
+      <c r="M25" s="11"/>
     </row>
     <row r="26" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18">
+      <c r="A26" s="10">
         <v>20</v>
       </c>
       <c r="B26" s="4"/>
@@ -1435,7 +1480,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="19"/>
+      <c r="M26" s="11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
feat: enhance UI and functionality across multiple pages
- Updated MaterialesPage, OrdersPage, ProveedoresPage, and ReceptionsPage to improve layout and styling with a consistent gradient background and enhanced headers.
- Refactored MaterialesPage and ProveedoresPage to integrate new MaterialList and SupplierList components with improved props for adding new items.
- Introduced LineDetailsAccordion and OrderDetailsAccordion components for better display of detailed information in consulta.
- Added Accordion and Badge components for improved UI consistency and usability.
- Updated Tailwind CSS configuration for better styling options and animations.
- Modified types to export ChangeHistoryItem interface for better type management.
</commit_message>
<xml_diff>
--- a/public/plantillas/int_excel_template.xlsx
+++ b/public/plantillas/int_excel_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\mat89\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E131DB8-3910-4539-A20F-57E8EE1390AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBCF5D7-3CA6-407D-A35B-74F4F148A6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A836C92A-72EE-4D4A-871D-9A1A52BD3A60}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>POS</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t xml:space="preserve">Taller Destino Reparacion:  </t>
-  </si>
-  <si>
-    <t>Base de Mantenimiento de Valencia - Alm. 140 + 141</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha Envio </t>
@@ -353,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -393,63 +390,59 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1008,7 +1001,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,61 +1022,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15"/>
-      <c r="B1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="J2" s="13" t="s">
+    <row r="2" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
+      <c r="F2" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="26"/>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="7"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -1131,28 +1115,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1535,66 +1519,66 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>